<commit_message>
13th commit Implemented CRUD minimal Api for customers
</commit_message>
<xml_diff>
--- a/LearnApiDemo/wwwroot/Export/customerinfo.xlsx
+++ b/LearnApiDemo/wwwroot/Export/customerinfo.xlsx
@@ -29,6 +29,18 @@
   </x:si>
   <x:si>
     <x:t>CreditLimit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ujjwal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ujwjal@in.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8787656789</x:t>
   </x:si>
   <x:si>
     <x:t>1</x:t>
@@ -104,8 +116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E2" totalsRowShown="0">
-  <x:autoFilter ref="A1:E2"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
+  <x:autoFilter ref="A1:E3"/>
   <x:tableColumns count="5">
     <x:tableColumn id="1" name="Code"/>
     <x:tableColumn id="2" name="Name"/>
@@ -405,7 +417,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:E3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -441,8 +453,25 @@
       <x:c r="D2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
+      <x:c r="E2" s="0">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>